<commit_message>
added sql statements and conditions
</commit_message>
<xml_diff>
--- a/dokumente/AchievementsList.xlsx
+++ b/dokumente/AchievementsList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\do-home1\Ext_SOPRA_Sauer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kickvinwl\dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Rookie</t>
   </si>
@@ -126,6 +126,75 @@
   </si>
   <si>
     <t>Tippspielsieger</t>
+  </si>
+  <si>
+    <t>SELECT count(mt.userPoints) FROM matchtip mt WHERE mt.fk_user = USERID</t>
+  </si>
+  <si>
+    <t>&gt;1</t>
+  </si>
+  <si>
+    <t>&gt;123</t>
+  </si>
+  <si>
+    <t>&gt;300</t>
+  </si>
+  <si>
+    <t>&gt;600</t>
+  </si>
+  <si>
+    <t>&gt;1234</t>
+  </si>
+  <si>
+    <t>Matchday mit count = 0</t>
+  </si>
+  <si>
+    <t>SELECT md.id, sum(mt.userPoints) FROM matchday md inner join matchtip mt on md.id=mt.fk_match WHERE mt.fk_user = USERID GROUP BY md.id</t>
+  </si>
+  <si>
+    <t>Matchday mt summe = 0</t>
+  </si>
+  <si>
+    <t>SELECT count(mt.id) from matchtip mt where mt.fk_user=USERID AND mt.userPoints = 4</t>
+  </si>
+  <si>
+    <t>SELECT count(mt.id) from matchday md inner join game g on g.matchdayId=md.id inner join matchtip mt on g.id=mt.fk_match where mt.fk_user=USERID AND mt.userPoints = 4 Group by md.id</t>
+  </si>
+  <si>
+    <t>SELECT md.id, count(mt.id) FROM  matchday md inner join game g on g.matchdayId=md.id inner join matchtip mt on g.id=mt.fk_match WHERE mt.fk_user = USERID AND mt.userPoints&lt;4 GROUP BY md.id</t>
+  </si>
+  <si>
+    <t>SELECT md.id, count(mt.id) FROM  matchday md inner join game g on g.matchdayId=md.id inner join matchtip mt on g.id=mt.fk_match WHERE mt.fk_user = USERID AND mt.userPoints&lt;1 GROUP BY md.id</t>
+  </si>
+  <si>
+    <t>count &gt; =5</t>
+  </si>
+  <si>
+    <t>count &gt; =3</t>
+  </si>
+  <si>
+    <t>count &gt; =1</t>
+  </si>
+  <si>
+    <t>Select mt.fk_user, sum(mt.userPoints) from matchtip mt inner join game g on mt.fk_match=g.id inner join matchday md inner join g.matchdayId=md.id group by mt.fk_user where md.id = MATCHDAYID Order by sum(mt.userPoints) Limit 1</t>
+  </si>
+  <si>
+    <t>Jeden Spieltag bekommt user mit dieser id das Achievement</t>
+  </si>
+  <si>
+    <t>default insert</t>
+  </si>
+  <si>
+    <t>Select mt.fk_user, sum(mt.userPoints) from matchtip mt inner join game g on mt.fk_match=g.id inner join matchday md inner join g.matchdayId=md.id inner join league l on md.leagueId=l.id group by mt.fk_user where l.id = leagueId Order by sum(mt.userPoints) Limit 1</t>
+  </si>
+  <si>
+    <t>untere abfrage mit allen League ids und dies dann zählen</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Erfüllt wenn</t>
   </si>
 </sst>
 </file>
@@ -457,152 +526,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="244.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added achiement query, some default data and achiement checker
</commit_message>
<xml_diff>
--- a/dokumente/AchievementsList.xlsx
+++ b/dokumente/AchievementsList.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kickvinwl\dokumente\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Rookie</t>
   </si>
@@ -128,24 +123,6 @@
     <t>Tippspielsieger</t>
   </si>
   <si>
-    <t>SELECT count(mt.userPoints) FROM matchtip mt WHERE mt.fk_user = USERID</t>
-  </si>
-  <si>
-    <t>&gt;1</t>
-  </si>
-  <si>
-    <t>&gt;123</t>
-  </si>
-  <si>
-    <t>&gt;300</t>
-  </si>
-  <si>
-    <t>&gt;600</t>
-  </si>
-  <si>
-    <t>&gt;1234</t>
-  </si>
-  <si>
     <t>Matchday mit count = 0</t>
   </si>
   <si>
@@ -195,13 +172,31 @@
   </si>
   <si>
     <t>Erfüllt wenn</t>
+  </si>
+  <si>
+    <t>SELECT mt.fk_user FROM matchtip mt GROUP BY fk_user HAVIN COUNT(mt.userPoints) &gt; 1</t>
+  </si>
+  <si>
+    <t>SELECT mt.fk_user FROM matchtip mt GROUP BY fk_user HAVIN COUNT(mt.userPoints) &gt; 123</t>
+  </si>
+  <si>
+    <t>SELECT mt.fk_user FROM matchtip mt GROUP BY fk_user HAVIN COUNT(mt.userPoints) &gt; 300</t>
+  </si>
+  <si>
+    <t>SELECT mt.fk_user FROM matchtip mt GROUP BY fk_user HAVIN COUNT(mt.userPoints) &gt; 600</t>
+  </si>
+  <si>
+    <t>SELECT mt.fk_user FROM matchtip mt GROUP BY fk_user HAVIN COUNT(mt.userPoints) &gt; 1234</t>
+  </si>
+  <si>
+    <t>NEED TO RETURN USER ID LIST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +207,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="48"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -238,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,6 +255,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -306,7 +317,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,7 +352,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,10 +559,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -562,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -573,10 +584,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -587,10 +595,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -601,10 +606,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -615,10 +617,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,10 +628,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -642,11 +638,11 @@
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="3" t="s">
         <v>40</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -656,11 +652,11 @@
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -670,11 +666,11 @@
       <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -684,11 +680,11 @@
       <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>48</v>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -698,11 +694,11 @@
       <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -712,11 +708,11 @@
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -726,12 +722,16 @@
       <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -740,9 +740,10 @@
       <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
+      <c r="C18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -751,9 +752,10 @@
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
+      <c r="C19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -762,11 +764,16 @@
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" t="s">
-        <v>51</v>
+      <c r="C20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="61.5" x14ac:dyDescent="0.9">
+      <c r="C24" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>